<commit_message>
import request - 9/10
- attempted different versions of pulling data to fix the summarized view
- found out there are dictionaries within the data pull that hold data
- NEXT STEPS: figure out a way to extract data from dictionaries seemlessly within the confines of the template already provided OR "Account Name": "value by time period" template
</commit_message>
<xml_diff>
--- a/balance_sheet.xlsx
+++ b/balance_sheet.xlsx
@@ -1,41 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03a4090e471ff419/Documents/GitHub/finevalgroup/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_08A501E0F613C866C1032425ED72D2AA75529535" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E2FAA63-B18A-4607-B550-80349DB5D746}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="39540" yWindow="4560" windowWidth="17250" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>TOTAL ASSETS</t>
-  </si>
-  <si>
-    <t>TOTAL LIABILITIES AND EQUITY</t>
-  </si>
-  <si>
-    <t>23436.29</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>{'ColData': [{'value': 'ASSETS'}, {'value': ''}]}</t>
+  </si>
+  <si>
+    <t>{'ColData': [{'value': 'LIABILITIES AND EQUITY'}, {'value': ''}]}</t>
+  </si>
+  <si>
+    <t>{'Row': [{'Header': {'ColData': [{'value': 'Current Assets'}, {'value': ''}]}, 'Rows': {'Row': [{'Header': {'ColData': [{'value': 'Bank Accounts'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Checking', 'id': '35'}, {'value': '1201.00'}], 'type': 'Data'}, {'ColData': [{'value': 'Savings', 'id': '36'}, {'value': '800.00'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Bank Accounts'}, {'value': '2001.00'}]}, 'type': 'Section', 'group': 'BankAccounts'}, {'Header': {'ColData': [{'value': 'Accounts Receivable'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Accounts Receivable (A/R)', 'id': '84'}, {'value': '5281.52'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Accounts Receivable'}, {'value': '5281.52'}]}, 'type': 'Section', 'group': 'AR'}, {'Header': {'ColData': [{'value': 'Other Current Assets'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Inventory Asset', 'id': '81'}, {'value': '596.25'}], 'type': 'Data'}, {'ColData': [{'value': 'Undeposited Funds', 'id': '4'}, {'value': '2062.52'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Other Current Assets'}, {'value': '2658.77'}]}, 'type': 'Section', 'group': 'OtherCurrentAssets'}]}, 'Summary': {'ColData': [{'value': 'Total Current Assets'}, {'value': '9941.29'}]}, 'type': 'Section', 'group': 'CurrentAssets'}, {'Header': {'ColData': [{'value': 'Fixed Assets'}, {'value': ''}]}, 'Rows': {'Row': [{'Header': {'ColData': [{'value': 'Truck', 'id': '37'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Original Cost', 'id': '38'}, {'value': '13495.00'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Truck'}, {'value': '13495.00'}]}, 'type': 'Section'}]}, 'Summary': {'ColData': [{'value': 'Total Fixed Assets'}, {'value': '13495.00'}]}, 'type': 'Section', 'group': 'FixedAssets'}]}</t>
+  </si>
+  <si>
+    <t>{'Row': [{'Header': {'ColData': [{'value': 'Liabilities'}, {'value': ''}]}, 'Rows': {'Row': [{'Header': {'ColData': [{'value': 'Current Liabilities'}, {'value': ''}]}, 'Rows': {'Row': [{'Header': {'ColData': [{'value': 'Accounts Payable'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Accounts Payable (A/P)', 'id': '33'}, {'value': '1602.67'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Accounts Payable'}, {'value': '1602.67'}]}, 'type': 'Section', 'group': 'AP'}, {'Header': {'ColData': [{'value': 'Credit Cards'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Mastercard', 'id': '41'}, {'value': '157.72'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Credit Cards'}, {'value': '157.72'}]}, 'type': 'Section', 'group': 'CreditCards'}, {'Header': {'ColData': [{'value': 'Other Current Liabilities'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Arizona Dept. of Revenue Payable', 'id': '89'}, {'value': '0.00'}], 'type': 'Data'}, {'ColData': [{'value': 'Board of Equalization Payable', 'id': '90'}, {'value': '370.94'}], 'type': 'Data'}, {'ColData': [{'value': 'Loan Payable', 'id': '43'}, {'value': '4000.00'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Other Current Liabilities'}, {'value': '4370.94'}]}, 'type': 'Section', 'group': 'OtherCurrentLiabilities'}]}, 'Summary': {'ColData': [{'value': 'Total Current Liabilities'}, {'value': '6131.33'}]}, 'type': 'Section', 'group': 'CurrentLiabilities'}, {'Header': {'ColData': [{'value': 'Long-Term Liabilities'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Notes Payable', 'id': '44'}, {'value': '25000.00'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Long-Term Liabilities'}, {'value': '25000.00'}]}, 'type': 'Section', 'group': 'LongTermLiabilities'}]}, 'Summary': {'ColData': [{'value': 'Total Liabilities'}, {'value': '31131.33'}]}, 'type': 'Section', 'group': 'Liabilities'}, {'Header': {'ColData': [{'value': 'Equity'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Opening Balance Equity', 'id': '34'}, {'value': '-9337.50'}], 'type': 'Data'}, {'ColData': [{'value': 'Retained Earnings', 'id': '2'}, {'value': ''}], 'type': 'Data'}, {'ColData': [{'value': 'Net Income'}, {'value': '1642.46'}], 'type': 'Data', 'group': 'NetIncome'}]}, 'Summary': {'ColData': [{'value': 'Total Equity'}, {'value': '-7695.04'}]}, 'type': 'Section', 'group': 'Equity'}]}</t>
+  </si>
+  <si>
+    <t>{'ColData': [{'value': 'TOTAL ASSETS'}, {'value': '23436.29'}]}</t>
+  </si>
+  <si>
+    <t>{'ColData': [{'value': 'TOTAL LIABILITIES AND EQUITY'}, {'value': '23436.29'}]}</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>TotalAssets</t>
+  </si>
+  <si>
+    <t>TotalLiabilitiesAndEquity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,13 +144,25 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -142,7 +200,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -176,6 +234,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -210,9 +269,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -385,35 +445,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="52.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
repass of balance sheet data pull
</commit_message>
<xml_diff>
--- a/balance_sheet.xlsx
+++ b/balance_sheet.xlsx
@@ -1,87 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03a4090e471ff419/Documents/GitHub/finevalgroup/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_08A501E0F613C866C1032425ED72D2AA75529535" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E2FAA63-B18A-4607-B550-80349DB5D746}"/>
   <bookViews>
-    <workbookView xWindow="39540" yWindow="4560" windowWidth="17250" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>Header</t>
-  </si>
-  <si>
-    <t>Rows</t>
-  </si>
-  <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>group</t>
-  </si>
-  <si>
-    <t>{'ColData': [{'value': 'ASSETS'}, {'value': ''}]}</t>
-  </si>
-  <si>
-    <t>{'ColData': [{'value': 'LIABILITIES AND EQUITY'}, {'value': ''}]}</t>
-  </si>
-  <si>
-    <t>{'Row': [{'Header': {'ColData': [{'value': 'Current Assets'}, {'value': ''}]}, 'Rows': {'Row': [{'Header': {'ColData': [{'value': 'Bank Accounts'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Checking', 'id': '35'}, {'value': '1201.00'}], 'type': 'Data'}, {'ColData': [{'value': 'Savings', 'id': '36'}, {'value': '800.00'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Bank Accounts'}, {'value': '2001.00'}]}, 'type': 'Section', 'group': 'BankAccounts'}, {'Header': {'ColData': [{'value': 'Accounts Receivable'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Accounts Receivable (A/R)', 'id': '84'}, {'value': '5281.52'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Accounts Receivable'}, {'value': '5281.52'}]}, 'type': 'Section', 'group': 'AR'}, {'Header': {'ColData': [{'value': 'Other Current Assets'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Inventory Asset', 'id': '81'}, {'value': '596.25'}], 'type': 'Data'}, {'ColData': [{'value': 'Undeposited Funds', 'id': '4'}, {'value': '2062.52'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Other Current Assets'}, {'value': '2658.77'}]}, 'type': 'Section', 'group': 'OtherCurrentAssets'}]}, 'Summary': {'ColData': [{'value': 'Total Current Assets'}, {'value': '9941.29'}]}, 'type': 'Section', 'group': 'CurrentAssets'}, {'Header': {'ColData': [{'value': 'Fixed Assets'}, {'value': ''}]}, 'Rows': {'Row': [{'Header': {'ColData': [{'value': 'Truck', 'id': '37'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Original Cost', 'id': '38'}, {'value': '13495.00'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Truck'}, {'value': '13495.00'}]}, 'type': 'Section'}]}, 'Summary': {'ColData': [{'value': 'Total Fixed Assets'}, {'value': '13495.00'}]}, 'type': 'Section', 'group': 'FixedAssets'}]}</t>
-  </si>
-  <si>
-    <t>{'Row': [{'Header': {'ColData': [{'value': 'Liabilities'}, {'value': ''}]}, 'Rows': {'Row': [{'Header': {'ColData': [{'value': 'Current Liabilities'}, {'value': ''}]}, 'Rows': {'Row': [{'Header': {'ColData': [{'value': 'Accounts Payable'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Accounts Payable (A/P)', 'id': '33'}, {'value': '1602.67'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Accounts Payable'}, {'value': '1602.67'}]}, 'type': 'Section', 'group': 'AP'}, {'Header': {'ColData': [{'value': 'Credit Cards'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Mastercard', 'id': '41'}, {'value': '157.72'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Credit Cards'}, {'value': '157.72'}]}, 'type': 'Section', 'group': 'CreditCards'}, {'Header': {'ColData': [{'value': 'Other Current Liabilities'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Arizona Dept. of Revenue Payable', 'id': '89'}, {'value': '0.00'}], 'type': 'Data'}, {'ColData': [{'value': 'Board of Equalization Payable', 'id': '90'}, {'value': '370.94'}], 'type': 'Data'}, {'ColData': [{'value': 'Loan Payable', 'id': '43'}, {'value': '4000.00'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Other Current Liabilities'}, {'value': '4370.94'}]}, 'type': 'Section', 'group': 'OtherCurrentLiabilities'}]}, 'Summary': {'ColData': [{'value': 'Total Current Liabilities'}, {'value': '6131.33'}]}, 'type': 'Section', 'group': 'CurrentLiabilities'}, {'Header': {'ColData': [{'value': 'Long-Term Liabilities'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Notes Payable', 'id': '44'}, {'value': '25000.00'}], 'type': 'Data'}]}, 'Summary': {'ColData': [{'value': 'Total Long-Term Liabilities'}, {'value': '25000.00'}]}, 'type': 'Section', 'group': 'LongTermLiabilities'}]}, 'Summary': {'ColData': [{'value': 'Total Liabilities'}, {'value': '31131.33'}]}, 'type': 'Section', 'group': 'Liabilities'}, {'Header': {'ColData': [{'value': 'Equity'}, {'value': ''}]}, 'Rows': {'Row': [{'ColData': [{'value': 'Opening Balance Equity', 'id': '34'}, {'value': '-9337.50'}], 'type': 'Data'}, {'ColData': [{'value': 'Retained Earnings', 'id': '2'}, {'value': ''}], 'type': 'Data'}, {'ColData': [{'value': 'Net Income'}, {'value': '1642.46'}], 'type': 'Data', 'group': 'NetIncome'}]}, 'Summary': {'ColData': [{'value': 'Total Equity'}, {'value': '-7695.04'}]}, 'type': 'Section', 'group': 'Equity'}]}</t>
-  </si>
-  <si>
-    <t>{'ColData': [{'value': 'TOTAL ASSETS'}, {'value': '23436.29'}]}</t>
-  </si>
-  <si>
-    <t>{'ColData': [{'value': 'TOTAL LIABILITIES AND EQUITY'}, {'value': '23436.29'}]}</t>
-  </si>
-  <si>
-    <t>Section</t>
-  </si>
-  <si>
-    <t>TotalAssets</t>
-  </si>
-  <si>
-    <t>TotalLiabilitiesAndEquity</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Checking</t>
+  </si>
+  <si>
+    <t>Accounts Receivable (A/R)</t>
+  </si>
+  <si>
+    <t>Inventory Asset</t>
+  </si>
+  <si>
+    <t>Notes Payable</t>
+  </si>
+  <si>
+    <t>1201.00</t>
+  </si>
+  <si>
+    <t>5281.52</t>
+  </si>
+  <si>
+    <t>596.25</t>
+  </si>
+  <si>
+    <t>25000.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,25 +113,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -200,7 +157,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -234,7 +191,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -269,10 +225,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -445,71 +400,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="52.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B5" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>